<commit_message>
Model comparison experiment, augmentation experiment and slight refactoring to training models and evaluation - removing need for specifying which split
</commit_message>
<xml_diff>
--- a/evaluation/results/isolation_forest/split_1/test_50_50/evaluation_metrics.xlsx
+++ b/evaluation/results/isolation_forest/split_1/test_50_50/evaluation_metrics.xlsx
@@ -500,37 +500,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="C2">
-        <v>0.8549848942598187</v>
+        <v>0.84</v>
       </c>
       <c r="D2">
-        <v>0.5299625468164794</v>
+        <v>0.5112359550561798</v>
       </c>
       <c r="E2">
-        <v>0.6543352601156069</v>
+        <v>0.6356228172293364</v>
       </c>
       <c r="F2">
-        <v>0.5735711390352655</v>
+        <v>0.5546525802519301</v>
       </c>
       <c r="G2">
-        <v>0.5378261822966157</v>
+        <v>0.5190493601462522</v>
       </c>
       <c r="H2">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="I2">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="J2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K2">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="L2">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -565,13 +565,13 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.6594301221166893</v>
+        <v>0.648721399730821</v>
       </c>
       <c r="C2">
-        <v>0.9101123595505618</v>
+        <v>0.9026217228464419</v>
       </c>
       <c r="D2">
-        <v>0.7647521636506688</v>
+        <v>0.754894283476899</v>
       </c>
       <c r="E2">
         <v>534</v>
@@ -582,13 +582,13 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.8549848942598187</v>
+        <v>0.84</v>
       </c>
       <c r="C3">
-        <v>0.5299625468164794</v>
+        <v>0.5112359550561798</v>
       </c>
       <c r="D3">
-        <v>0.6543352601156069</v>
+        <v>0.6356228172293364</v>
       </c>
       <c r="E3">
         <v>534</v>
@@ -599,16 +599,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="C4">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="D4">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="E4">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -616,13 +616,13 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>0.757207508188254</v>
+        <v>0.7443606998654104</v>
       </c>
       <c r="C5">
-        <v>0.7200374531835205</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="D5">
-        <v>0.7095437118831378</v>
+        <v>0.6952585503531177</v>
       </c>
       <c r="E5">
         <v>1068</v>
@@ -633,13 +633,13 @@
         <v>21</v>
       </c>
       <c r="B6">
-        <v>0.757207508188254</v>
+        <v>0.7443606998654104</v>
       </c>
       <c r="C6">
-        <v>0.7200374531835206</v>
+        <v>0.7069288389513109</v>
       </c>
       <c r="D6">
-        <v>0.7095437118831378</v>
+        <v>0.6952585503531178</v>
       </c>
       <c r="E6">
         <v>1068</v>
@@ -671,10 +671,10 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C2">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -682,10 +682,10 @@
         <v>25</v>
       </c>
       <c r="B3">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C3">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hybrid model working with complete evaluation, refactoring done to scaler storage and loading, training+evaluation pipeline script complete
</commit_message>
<xml_diff>
--- a/evaluation/results/isolation_forest/split_1/test_50_50/evaluation_metrics.xlsx
+++ b/evaluation/results/isolation_forest/split_1/test_50_50/evaluation_metrics.xlsx
@@ -500,37 +500,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="C2">
-        <v>0.84</v>
+        <v>0.9244604316546763</v>
       </c>
       <c r="D2">
-        <v>0.5112359550561798</v>
+        <v>0.4812734082397004</v>
       </c>
       <c r="E2">
-        <v>0.6356228172293364</v>
+        <v>0.6330049261083743</v>
       </c>
       <c r="F2">
-        <v>0.5546525802519301</v>
+        <v>0.5323115161557581</v>
       </c>
       <c r="G2">
-        <v>0.5190493601462522</v>
+        <v>0.4903140592896977</v>
       </c>
       <c r="H2">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715357</v>
       </c>
       <c r="I2">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="J2">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="K2">
-        <v>482</v>
+        <v>513</v>
       </c>
       <c r="L2">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -565,13 +565,13 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.648721399730821</v>
+        <v>0.649367088607595</v>
       </c>
       <c r="C2">
-        <v>0.9026217228464419</v>
+        <v>0.9606741573033708</v>
       </c>
       <c r="D2">
-        <v>0.754894283476899</v>
+        <v>0.7749244712990937</v>
       </c>
       <c r="E2">
         <v>534</v>
@@ -582,13 +582,13 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.84</v>
+        <v>0.9244604316546763</v>
       </c>
       <c r="C3">
-        <v>0.5112359550561798</v>
+        <v>0.4812734082397004</v>
       </c>
       <c r="D3">
-        <v>0.6356228172293364</v>
+        <v>0.6330049261083743</v>
       </c>
       <c r="E3">
         <v>534</v>
@@ -599,16 +599,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="C4">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="D4">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="E4">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -616,13 +616,13 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>0.7443606998654104</v>
+        <v>0.7869137601311356</v>
       </c>
       <c r="C5">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="D5">
-        <v>0.6952585503531177</v>
+        <v>0.703964698703734</v>
       </c>
       <c r="E5">
         <v>1068</v>
@@ -633,13 +633,13 @@
         <v>21</v>
       </c>
       <c r="B6">
-        <v>0.7443606998654104</v>
+        <v>0.7869137601311357</v>
       </c>
       <c r="C6">
-        <v>0.7069288389513109</v>
+        <v>0.7209737827715356</v>
       </c>
       <c r="D6">
-        <v>0.6952585503531178</v>
+        <v>0.703964698703734</v>
       </c>
       <c r="E6">
         <v>1068</v>
@@ -671,10 +671,10 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>482</v>
+        <v>513</v>
       </c>
       <c r="C2">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -682,10 +682,10 @@
         <v>25</v>
       </c>
       <c r="B3">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="C3">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>